<commit_message>
Correction to f-gas calculations in indst/BPEiC
</commit_message>
<xml_diff>
--- a/InputData/indst/BPEiC/BAU Process Emis in CO2e.xlsx
+++ b/InputData/indst/BPEiC/BAU Process Emis in CO2e.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\US States\eps-california\InputData\indst\BPEiC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53F97DB-5F49-4E54-97FA-DF2F134108A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA947255-83A2-41CB-81AE-1E51A50A75B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3270" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -425,13 +425,13 @@
     <t>F-gases are estimated based on historic CARB data and E3's reference scenario projections for 2030 and 2050.</t>
   </si>
   <si>
-    <t>E3 Estimates for Trend Calibration</t>
-  </si>
-  <si>
     <t>Trend Estimation and Calibration</t>
   </si>
   <si>
     <t>Non-ODS Total</t>
+  </si>
+  <si>
+    <t>E3 Estimates for ODS Trend Calibration</t>
   </si>
 </sst>
 </file>
@@ -734,7 +734,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -742,6 +741,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="3" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
@@ -1054,11 +1054,11 @@
                 <c:pt idx="18">
                   <c:v>20.149999999999999</c:v>
                 </c:pt>
-                <c:pt idx="19">
-                  <c:v>23.4</c:v>
+                <c:pt idx="19" formatCode="0.00">
+                  <c:v>23.287599999999998</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>30.6</c:v>
+                <c:pt idx="20" formatCode="0.00">
+                  <c:v>30.497600000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5116,7 +5116,7 @@
     </row>
     <row r="31" spans="1:15" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A31" s="17"/>
-      <c r="B31" s="56"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
       <c r="E31" s="17"/>
@@ -5190,7 +5190,7 @@
     </row>
     <row r="35" spans="1:15" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
-      <c r="B35" s="57" t="s">
+      <c r="B35" s="56" t="s">
         <v>106</v>
       </c>
       <c r="C35" s="17"/>
@@ -6455,7 +6455,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -6562,7 +6562,7 @@
         <f>About!$C$52</f>
         <v>0</v>
       </c>
-      <c r="E3" s="58">
+      <c r="E3" s="57">
         <f>'CARB 2020_F-gases'!T8*1000000000000</f>
         <v>20150000000000</v>
       </c>
@@ -6575,7 +6575,7 @@
       <c r="H3" s="7">
         <v>0</v>
       </c>
-      <c r="I3" s="58">
+      <c r="I3" s="57">
         <f>'CARB 2020_F-gases'!T12*1000000000000</f>
         <v>310000000000.00006</v>
       </c>
@@ -6613,7 +6613,7 @@
       </c>
       <c r="E4" s="7">
         <f t="array" ref="E4:E35">TRANSPOSE('CARB 2020_F-gases'!B17:AG17)*1000000000000</f>
-        <v>20015400000000</v>
+        <v>19972900000000</v>
       </c>
       <c r="F4" s="7">
         <v>0</v>
@@ -6661,7 +6661,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="7">
-        <v>20634700000000</v>
+        <v>20587600000000</v>
       </c>
       <c r="F5" s="7">
         <v>0</v>
@@ -6708,7 +6708,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="7">
-        <v>21234800000000</v>
+        <v>21182900000000</v>
       </c>
       <c r="F6" s="7">
         <v>0</v>
@@ -6755,7 +6755,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="7">
-        <v>21815700000000</v>
+        <v>21758800000000</v>
       </c>
       <c r="F7" s="7">
         <v>0</v>
@@ -6802,7 +6802,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="7">
-        <v>22377399999999.996</v>
+        <v>22315300000000</v>
       </c>
       <c r="F8" s="7">
         <v>0</v>
@@ -6849,7 +6849,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="7">
-        <v>22919900000000</v>
+        <v>22852400000000</v>
       </c>
       <c r="F9" s="7">
         <v>0</v>
@@ -6896,7 +6896,7 @@
         <v>0</v>
       </c>
       <c r="E10" s="7">
-        <v>23443199999999.996</v>
+        <v>23370100000000</v>
       </c>
       <c r="F10" s="7">
         <v>0</v>
@@ -6943,7 +6943,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="7">
-        <v>23947300000000</v>
+        <v>23868399999999.996</v>
       </c>
       <c r="F11" s="7">
         <v>0</v>
@@ -6990,7 +6990,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="7">
-        <v>24432200000000</v>
+        <v>24347300000000</v>
       </c>
       <c r="F12" s="7">
         <v>0</v>
@@ -7037,7 +7037,7 @@
         <v>0</v>
       </c>
       <c r="E13" s="7">
-        <v>24897900000000</v>
+        <v>24806800000000.004</v>
       </c>
       <c r="F13" s="7">
         <v>0</v>
@@ -7084,7 +7084,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="7">
-        <v>25344400000000</v>
+        <v>25246900000000</v>
       </c>
       <c r="F14" s="7">
         <v>0</v>
@@ -7131,7 +7131,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="7">
-        <v>25771700000000</v>
+        <v>25667600000000</v>
       </c>
       <c r="F15" s="7">
         <v>0</v>
@@ -7178,7 +7178,7 @@
         <v>0</v>
       </c>
       <c r="E16" s="7">
-        <v>26179800000000</v>
+        <v>26068900000000</v>
       </c>
       <c r="F16" s="7">
         <v>0</v>
@@ -7225,7 +7225,7 @@
         <v>0</v>
       </c>
       <c r="E17" s="7">
-        <v>26568700000000</v>
+        <v>26450800000000</v>
       </c>
       <c r="F17" s="7">
         <v>0</v>
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
       <c r="E18" s="7">
-        <v>26938399999999.996</v>
+        <v>26813300000000</v>
       </c>
       <c r="F18" s="7">
         <v>0</v>
@@ -7319,7 +7319,7 @@
         <v>0</v>
       </c>
       <c r="E19" s="7">
-        <v>27288900000000</v>
+        <v>27156399999999.996</v>
       </c>
       <c r="F19" s="7">
         <v>0</v>
@@ -7366,7 +7366,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="7">
-        <v>27620199999999.996</v>
+        <v>27480099999999.996</v>
       </c>
       <c r="F20" s="7">
         <v>0</v>
@@ -7413,7 +7413,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="7">
-        <v>27932300000000</v>
+        <v>27784399999999.996</v>
       </c>
       <c r="F21" s="7">
         <v>0</v>
@@ -7460,7 +7460,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="7">
-        <v>28225199999999.992</v>
+        <v>28069300000000</v>
       </c>
       <c r="F22" s="7">
         <v>0</v>
@@ -7507,7 +7507,7 @@
         <v>0</v>
       </c>
       <c r="E23" s="7">
-        <v>28498900000000</v>
+        <v>28334799999999.996</v>
       </c>
       <c r="F23" s="7">
         <v>0</v>
@@ -7554,7 +7554,7 @@
         <v>0</v>
       </c>
       <c r="E24" s="7">
-        <v>28753400000000</v>
+        <v>28580899999999.996</v>
       </c>
       <c r="F24" s="7">
         <v>0</v>
@@ -7601,7 +7601,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="7">
-        <v>28988699999999.996</v>
+        <v>28807600000000</v>
       </c>
       <c r="F25" s="7">
         <v>0</v>
@@ -7648,7 +7648,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="7">
-        <v>29204799999999.996</v>
+        <v>29014900000000</v>
       </c>
       <c r="F26" s="7">
         <v>0</v>
@@ -7695,7 +7695,7 @@
         <v>0</v>
       </c>
       <c r="E27" s="7">
-        <v>29401700000000</v>
+        <v>29202800000000</v>
       </c>
       <c r="F27" s="7">
         <v>0</v>
@@ -7742,7 +7742,7 @@
         <v>0</v>
       </c>
       <c r="E28" s="7">
-        <v>29579400000000</v>
+        <v>29371300000000</v>
       </c>
       <c r="F28" s="7">
         <v>0</v>
@@ -7789,7 +7789,7 @@
         <v>0</v>
       </c>
       <c r="E29" s="7">
-        <v>29737899999999.996</v>
+        <v>29520400000000</v>
       </c>
       <c r="F29" s="7">
         <v>0</v>
@@ -7836,7 +7836,7 @@
         <v>0</v>
       </c>
       <c r="E30" s="7">
-        <v>29877200000000</v>
+        <v>29650100000000</v>
       </c>
       <c r="F30" s="7">
         <v>0</v>
@@ -7883,7 +7883,7 @@
         <v>0</v>
       </c>
       <c r="E31" s="7">
-        <v>29997300000000</v>
+        <v>29760400000000</v>
       </c>
       <c r="F31" s="7">
         <v>0</v>
@@ -7930,7 +7930,7 @@
         <v>0</v>
       </c>
       <c r="E32" s="7">
-        <v>30098199999999.996</v>
+        <v>29851300000000</v>
       </c>
       <c r="F32" s="7">
         <v>0</v>
@@ -7977,7 +7977,7 @@
         <v>0</v>
       </c>
       <c r="E33" s="7">
-        <v>30179899999999.996</v>
+        <v>29922800000000</v>
       </c>
       <c r="F33" s="7">
         <v>0</v>
@@ -8024,7 +8024,7 @@
         <v>0</v>
       </c>
       <c r="E34" s="7">
-        <v>30242400000000</v>
+        <v>29974900000000</v>
       </c>
       <c r="F34" s="7">
         <v>0</v>
@@ -8071,7 +8071,7 @@
         <v>0</v>
       </c>
       <c r="E35" s="7">
-        <v>30285700000000.004</v>
+        <v>30007599999999.996</v>
       </c>
       <c r="F35" s="7">
         <v>0</v>
@@ -18950,7 +18950,9 @@
   </sheetPr>
   <dimension ref="A1:AG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -18959,7 +18961,7 @@
     <col min="3" max="3" width="9.796875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.9296875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.9296875" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.6640625" customWidth="1"/>
+    <col min="21" max="22" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.45">
@@ -18978,32 +18980,32 @@
       </c>
     </row>
     <row r="5" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="53" t="s">
+      <c r="A5" s="52" t="s">
         <v>95</v>
       </c>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
-      <c r="H5" s="52"/>
-      <c r="I5" s="52"/>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="52"/>
-      <c r="O5" s="52"/>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="55" t="s">
-        <v>110</v>
-      </c>
-      <c r="V5" s="54"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="51"/>
+      <c r="I5" s="51"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="51"/>
+      <c r="L5" s="51"/>
+      <c r="M5" s="51"/>
+      <c r="N5" s="51"/>
+      <c r="O5" s="51"/>
+      <c r="P5" s="51"/>
+      <c r="Q5" s="51"/>
+      <c r="R5" s="51"/>
+      <c r="S5" s="51"/>
+      <c r="T5" s="51"/>
+      <c r="U5" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="V5" s="53"/>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.45">
       <c r="A6" s="25" t="s">
@@ -19204,13 +19206,13 @@
       <c r="T8">
         <v>20.149999999999999</v>
       </c>
-      <c r="U8" s="51">
-        <f>B70</f>
-        <v>23.4</v>
-      </c>
-      <c r="V8" s="51">
-        <f>B71</f>
-        <v>30.6</v>
+      <c r="U8" s="58">
+        <f>B70-SUM(M18:M19)</f>
+        <v>23.287599999999998</v>
+      </c>
+      <c r="V8" s="58">
+        <f>B71-SUM(AG18:AG19)</f>
+        <v>30.497600000000002</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.45">
@@ -19340,7 +19342,7 @@
     <row r="11" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="12" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" s="19">
         <f>SUM(B9:B10)</f>
@@ -19423,41 +19425,41 @@
       <c r="A13" s="26"/>
     </row>
     <row r="14" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="53" t="s">
+      <c r="A14" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="52"/>
-      <c r="L14" s="52"/>
-      <c r="M14" s="52"/>
-      <c r="N14" s="52"/>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="52"/>
-      <c r="S14" s="52"/>
-      <c r="T14" s="52"/>
-      <c r="U14" s="52"/>
-      <c r="V14" s="52"/>
-      <c r="W14" s="52"/>
-      <c r="X14" s="52"/>
-      <c r="Y14" s="52"/>
-      <c r="Z14" s="52"/>
-      <c r="AA14" s="52"/>
-      <c r="AB14" s="52"/>
-      <c r="AC14" s="52"/>
-      <c r="AD14" s="52"/>
-      <c r="AE14" s="52"/>
-      <c r="AF14" s="52"/>
-      <c r="AG14" s="52"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="51"/>
+      <c r="K14" s="51"/>
+      <c r="L14" s="51"/>
+      <c r="M14" s="51"/>
+      <c r="N14" s="51"/>
+      <c r="O14" s="51"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="51"/>
+      <c r="R14" s="51"/>
+      <c r="S14" s="51"/>
+      <c r="T14" s="51"/>
+      <c r="U14" s="51"/>
+      <c r="V14" s="51"/>
+      <c r="W14" s="51"/>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="51"/>
+      <c r="Z14" s="51"/>
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="51"/>
+      <c r="AE14" s="51"/>
+      <c r="AF14" s="51"/>
+      <c r="AG14" s="51"/>
     </row>
     <row r="15" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A15" s="25" t="s">
@@ -19667,131 +19669,131 @@
       </c>
       <c r="B17" s="19">
         <f>$B$25*B16^2+$B$26*B16+$B$27</f>
-        <v>20.0154</v>
+        <v>19.972899999999999</v>
       </c>
       <c r="C17" s="19">
         <f t="shared" ref="C17:AG17" si="1">$B$25*C16^2+$B$26*C16+$B$27</f>
-        <v>20.634699999999999</v>
+        <v>20.587600000000002</v>
       </c>
       <c r="D17" s="19">
         <f t="shared" si="1"/>
-        <v>21.2348</v>
+        <v>21.1829</v>
       </c>
       <c r="E17" s="19">
         <f t="shared" si="1"/>
-        <v>21.8157</v>
+        <v>21.758800000000001</v>
       </c>
       <c r="F17" s="19">
         <f t="shared" si="1"/>
-        <v>22.377399999999998</v>
+        <v>22.315300000000001</v>
       </c>
       <c r="G17" s="19">
         <f t="shared" si="1"/>
-        <v>22.919899999999998</v>
+        <v>22.852399999999999</v>
       </c>
       <c r="H17" s="19">
         <f t="shared" si="1"/>
-        <v>23.443199999999997</v>
+        <v>23.370100000000001</v>
       </c>
       <c r="I17" s="19">
         <f t="shared" si="1"/>
-        <v>23.947299999999998</v>
+        <v>23.868399999999998</v>
       </c>
       <c r="J17" s="19">
         <f t="shared" si="1"/>
-        <v>24.432199999999998</v>
+        <v>24.347300000000001</v>
       </c>
       <c r="K17" s="19">
         <f t="shared" si="1"/>
-        <v>24.8979</v>
+        <v>24.806800000000003</v>
       </c>
       <c r="L17" s="19">
         <f t="shared" si="1"/>
-        <v>25.3444</v>
+        <v>25.2469</v>
       </c>
       <c r="M17" s="19">
         <f t="shared" si="1"/>
-        <v>25.771699999999999</v>
+        <v>25.6676</v>
       </c>
       <c r="N17" s="19">
         <f t="shared" si="1"/>
-        <v>26.1798</v>
+        <v>26.068899999999999</v>
       </c>
       <c r="O17" s="19">
         <f t="shared" si="1"/>
-        <v>26.5687</v>
+        <v>26.450800000000001</v>
       </c>
       <c r="P17" s="19">
         <f t="shared" si="1"/>
-        <v>26.938399999999994</v>
+        <v>26.813299999999998</v>
       </c>
       <c r="Q17" s="19">
         <f t="shared" si="1"/>
-        <v>27.288899999999998</v>
+        <v>27.156399999999998</v>
       </c>
       <c r="R17" s="19">
         <f t="shared" si="1"/>
-        <v>27.620199999999997</v>
+        <v>27.480099999999997</v>
       </c>
       <c r="S17" s="19">
         <f t="shared" si="1"/>
-        <v>27.932300000000001</v>
+        <v>27.784399999999998</v>
       </c>
       <c r="T17" s="19">
         <f t="shared" si="1"/>
-        <v>28.225199999999994</v>
+        <v>28.069299999999998</v>
       </c>
       <c r="U17" s="19">
         <f t="shared" si="1"/>
-        <v>28.498899999999999</v>
+        <v>28.334799999999994</v>
       </c>
       <c r="V17" s="19">
         <f t="shared" si="1"/>
-        <v>28.753399999999999</v>
+        <v>28.580899999999996</v>
       </c>
       <c r="W17" s="19">
         <f t="shared" si="1"/>
-        <v>28.988699999999994</v>
+        <v>28.807600000000001</v>
       </c>
       <c r="X17" s="19">
         <f t="shared" si="1"/>
-        <v>29.204799999999995</v>
+        <v>29.014900000000001</v>
       </c>
       <c r="Y17" s="19">
         <f t="shared" si="1"/>
-        <v>29.401699999999998</v>
+        <v>29.2028</v>
       </c>
       <c r="Z17" s="19">
         <f t="shared" si="1"/>
-        <v>29.5794</v>
+        <v>29.371300000000002</v>
       </c>
       <c r="AA17" s="19">
         <f t="shared" si="1"/>
-        <v>29.737899999999996</v>
+        <v>29.520399999999999</v>
       </c>
       <c r="AB17" s="19">
         <f t="shared" si="1"/>
-        <v>29.877199999999998</v>
+        <v>29.650099999999998</v>
       </c>
       <c r="AC17" s="19">
         <f t="shared" si="1"/>
-        <v>29.997299999999999</v>
+        <v>29.760400000000001</v>
       </c>
       <c r="AD17" s="19">
         <f t="shared" si="1"/>
-        <v>30.098199999999995</v>
+        <v>29.851299999999998</v>
       </c>
       <c r="AE17" s="19">
         <f t="shared" si="1"/>
-        <v>30.179899999999996</v>
+        <v>29.922799999999999</v>
       </c>
       <c r="AF17" s="19">
         <f t="shared" si="1"/>
-        <v>30.2424</v>
+        <v>29.974899999999998</v>
       </c>
       <c r="AG17" s="19">
         <f t="shared" si="1"/>
-        <v>30.285700000000002</v>
+        <v>30.007599999999996</v>
       </c>
     </row>
     <row r="18" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
@@ -20065,7 +20067,7 @@
     </row>
     <row r="21" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B21" s="19">
         <f>SUM(B18:B19)</f>
@@ -20200,41 +20202,41 @@
       <c r="A22" s="26"/>
     </row>
     <row r="23" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="B23" s="52"/>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="52"/>
-      <c r="G23" s="52"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="52"/>
-      <c r="J23" s="52"/>
-      <c r="K23" s="52"/>
-      <c r="L23" s="52"/>
-      <c r="M23" s="52"/>
-      <c r="N23" s="52"/>
-      <c r="O23" s="52"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="52"/>
-      <c r="R23" s="52"/>
-      <c r="S23" s="52"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="52"/>
-      <c r="V23" s="52"/>
-      <c r="W23" s="52"/>
-      <c r="X23" s="52"/>
-      <c r="Y23" s="52"/>
-      <c r="Z23" s="52"/>
-      <c r="AA23" s="52"/>
-      <c r="AB23" s="52"/>
-      <c r="AC23" s="52"/>
-      <c r="AD23" s="52"/>
-      <c r="AE23" s="52"/>
-      <c r="AF23" s="52"/>
-      <c r="AG23" s="52"/>
+      <c r="A23" s="52" t="s">
+        <v>110</v>
+      </c>
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="51"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="51"/>
+      <c r="M23" s="51"/>
+      <c r="N23" s="51"/>
+      <c r="O23" s="51"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="51"/>
+      <c r="R23" s="51"/>
+      <c r="S23" s="51"/>
+      <c r="T23" s="51"/>
+      <c r="U23" s="51"/>
+      <c r="V23" s="51"/>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
+      <c r="AB23" s="51"/>
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+      <c r="AE23" s="51"/>
+      <c r="AF23" s="51"/>
+      <c r="AG23" s="51"/>
     </row>
     <row r="24" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="26" t="s">
@@ -20252,7 +20254,7 @@
         <v>97</v>
       </c>
       <c r="B25" s="19">
-        <v>-9.5999999999999992E-3</v>
+        <v>-9.7000000000000003E-3</v>
       </c>
       <c r="G25" s="26" t="s">
         <v>100</v>
@@ -20272,7 +20274,7 @@
         <v>98</v>
       </c>
       <c r="B26" s="19">
-        <v>1.0128999999999999</v>
+        <v>1.0124</v>
       </c>
       <c r="G26" s="26" t="s">
         <v>99</v>
@@ -20292,7 +20294,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="19">
-        <v>3.5973999999999999</v>
+        <v>3.6049000000000002</v>
       </c>
     </row>
     <row r="29" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Updated coefficient terminology for F-gas trend calculations in indst/BPEiC
</commit_message>
<xml_diff>
--- a/InputData/indst/BPEiC/BAU Process Emis in CO2e.xlsx
+++ b/InputData/indst/BPEiC/BAU Process Emis in CO2e.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\Documents\Energy Policy Simulator\Models\US States\eps-california\InputData\indst\BPEiC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA947255-83A2-41CB-81AE-1E51A50A75B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6470A5C-5079-4547-BBFA-5D82E1013024}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="3270" windowWidth="29040" windowHeight="17640" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="112">
   <si>
     <t>BPEiC BAU Process Emissions in CO2e</t>
   </si>
@@ -386,18 +386,6 @@
     <t>Future Year Projections</t>
   </si>
   <si>
-    <t>Leading Coefficient</t>
-  </si>
-  <si>
-    <t>Second Coefficient</t>
-  </si>
-  <si>
-    <t>Constant</t>
-  </si>
-  <si>
-    <t>Coefficient</t>
-  </si>
-  <si>
     <t>ODS Trend Estimation</t>
   </si>
   <si>
@@ -432,6 +420,15 @@
   </si>
   <si>
     <t>E3 Estimates for ODS Trend Calibration</t>
+  </si>
+  <si>
+    <t>Second Order Coefficient</t>
+  </si>
+  <si>
+    <t>First Order Coefficient</t>
+  </si>
+  <si>
+    <t>Zero Order Coefficient</t>
   </si>
 </sst>
 </file>
@@ -5134,7 +5131,7 @@
     <row r="32" spans="1:15" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A32" s="17"/>
       <c r="B32" s="11" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C32" s="17"/>
       <c r="D32" s="17"/>
@@ -5172,7 +5169,7 @@
     <row r="34" spans="1:15" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A34" s="17"/>
       <c r="B34" s="11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C34" s="17"/>
       <c r="D34" s="17"/>
@@ -5191,7 +5188,7 @@
     <row r="35" spans="1:15" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A35" s="17"/>
       <c r="B35" s="56" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="C35" s="17"/>
       <c r="D35" s="17"/>
@@ -5210,7 +5207,7 @@
     <row r="36" spans="1:15" s="19" customFormat="1" ht="14.25" x14ac:dyDescent="0.45">
       <c r="A36" s="17"/>
       <c r="B36" s="11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="C36" s="17"/>
       <c r="D36" s="17"/>
@@ -5445,7 +5442,7 @@
     </row>
     <row r="50" spans="1:15" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A50" s="44" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="B50" s="17"/>
       <c r="C50" s="17"/>
@@ -18950,9 +18947,7 @@
   </sheetPr>
   <dimension ref="A1:AG71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -19003,7 +18998,7 @@
       <c r="S5" s="51"/>
       <c r="T5" s="51"/>
       <c r="U5" s="54" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="V5" s="53"/>
     </row>
@@ -19342,7 +19337,7 @@
     <row r="11" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="12" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A12" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B12" s="19">
         <f>SUM(B9:B10)</f>
@@ -20067,7 +20062,7 @@
     </row>
     <row r="21" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A21" s="26" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B21" s="19">
         <f>SUM(B18:B19)</f>
@@ -20203,7 +20198,7 @@
     </row>
     <row r="23" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A23" s="52" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B23" s="51"/>
       <c r="C23" s="51"/>
@@ -20240,30 +20235,30 @@
     </row>
     <row r="24" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A24" s="26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G24" s="26" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="N24" s="26" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A25" s="26" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B25" s="19">
         <v>-9.7000000000000003E-3</v>
       </c>
       <c r="G25" s="26" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="H25" s="19">
         <v>-2.06E-2</v>
       </c>
       <c r="N25" s="26" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="O25" s="19">
         <v>-5.0000000000000001E-4</v>
@@ -20271,19 +20266,19 @@
     </row>
     <row r="26" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A26" s="26" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="B26" s="19">
         <v>1.0124</v>
       </c>
       <c r="G26" s="26" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="H26" s="19">
         <v>0.49909999999999999</v>
       </c>
       <c r="N26" s="26" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="O26" s="19">
         <v>0.12790000000000001</v>
@@ -20291,7 +20286,7 @@
     </row>
     <row r="27" spans="1:33" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A27" s="26" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B27" s="19">
         <v>3.6049000000000002</v>
@@ -20316,7 +20311,7 @@
     <row r="45" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.45"/>
     <row r="46" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A46" s="26" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:1" s="19" customFormat="1" x14ac:dyDescent="0.45"/>

</xml_diff>